<commit_message>
moving paper files into separate folder
</commit_message>
<xml_diff>
--- a/doc/voyager_lism_lit_review.xlsx
+++ b/doc/voyager_lism_lit_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\sf_gap_analysis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2314DBA7-1518-449C-84DC-5105EAA6943F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A310A-80D0-4DDC-8A8D-58CEE4C40B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-11385" windowWidth="29040" windowHeight="15720" xr2:uid="{744BB5EC-7CDC-4C43-818F-74C8129A6F6E}"/>
+    <workbookView xWindow="-25320" yWindow="-2025" windowWidth="25440" windowHeight="15270" xr2:uid="{744BB5EC-7CDC-4C43-818F-74C8129A6F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Interval</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>L1</t>
-  </si>
-  <si>
-    <t>Generallym, but not always, analyse stationary ("quiet") ints</t>
   </si>
   <si>
     <t>Interval length (days)</t>
@@ -150,9 +147,6 @@
     <t>W2</t>
   </si>
   <si>
-    <t>I1</t>
-  </si>
-  <si>
     <t>I3</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
   </si>
   <si>
     <t>Integral of power spectrum</t>
-  </si>
-  <si>
-    <t>Taylor scale (km)</t>
   </si>
   <si>
     <t>5000/0.048</t>
@@ -263,6 +254,45 @@
       </rPr>
       <t>not LISM)</t>
     </r>
+  </si>
+  <si>
+    <t>and others in text</t>
+  </si>
+  <si>
+    <t>Generally, but not always, analyse stationary ("quiet") ints</t>
+  </si>
+  <si>
+    <t>Tasnim</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>1977-2018</t>
+  </si>
+  <si>
+    <t>Radial study using 10 hour intervals, including (velocity) corr length</t>
+  </si>
+  <si>
+    <t>Taylor scale (km/hr)</t>
+  </si>
+  <si>
+    <t>30-50 days around 2014 shock (sh1)</t>
+  </si>
+  <si>
+    <t>PDFs and intermittency, power spectra</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>Kolmogorov at small scales, shallower at large scales</t>
+  </si>
+  <si>
+    <t>2019-2019</t>
+  </si>
+  <si>
+    <t>(same as 2015)</t>
   </si>
 </sst>
 </file>
@@ -372,21 +402,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -400,6 +426,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F722E8-72DA-4AAE-ABFC-BC8E13E2834D}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,124 +792,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="A3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
+      <c r="K4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="N4" s="13"/>
+      <c r="O4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="8" t="s">
+      <c r="P4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="8" t="s">
+      <c r="R4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="U4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -888,14 +917,14 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
+      <c r="D5" s="4">
+        <v>2013</v>
       </c>
       <c r="E5">
         <v>468</v>
@@ -913,36 +942,39 @@
         <v>2.9999999999999999E-7</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Q5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D6" s="6" t="s">
-        <v>34</v>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="E6">
         <v>466</v>
@@ -955,11 +987,11 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -983,7 +1015,7 @@
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K7">
         <v>0.36</v>
@@ -998,18 +1030,18 @@
         <v>5000000</v>
       </c>
       <c r="O7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E8">
         <v>468</v>
@@ -1020,6 +1052,9 @@
       <c r="G8">
         <v>-1.65</v>
       </c>
+      <c r="H8" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="K8">
         <v>0.28000000000000003</v>
       </c>
@@ -1033,21 +1068,21 @@
         <v>5000000</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>227</v>
@@ -1071,15 +1106,15 @@
         <v>5000000</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D10" s="6" t="s">
-        <v>39</v>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="E10">
         <v>466</v>
@@ -1103,29 +1138,29 @@
         <v>5000000</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="R10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <v>256</v>
       </c>
       <c r="P11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12">
         <v>365</v>
@@ -1139,115 +1174,185 @@
         <v>57.870370370370374</v>
       </c>
       <c r="P12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="M13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>60</v>
+      <c r="B13" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>2025</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15">
+        <v>285</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>32</v>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16">
+        <f>365+178-75</f>
+        <v>468</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="2">
-        <v>2014</v>
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>2023</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>54</v>
+      <c r="D20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="B23">
+      <c r="B26">
         <v>2023</v>
       </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>55</v>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>14</v>
+      <c r="E27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28">
+        <v>2020</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>21</v>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B1:P2"/>
+    <mergeCell ref="A3:E3"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
@@ -1255,8 +1360,6 @@
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="B1:P2"/>
-    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D10">
     <cfRule type="uniqueValues" priority="3"/>
@@ -1287,11 +1390,14 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://iopscience.iop.org/article/10.3847/1538-4357/aafd30/meta" xr:uid="{78750883-3C07-4AFA-8C6B-A4CB77ADDF1A}"/>
-    <hyperlink ref="B20" r:id="rId2" display="https://iopscience.iop.org/article/10.1088/0004-637X/792/2/134/pdf" xr:uid="{61E00B74-8AA3-4F56-8D64-5040CF6273FD}"/>
-    <hyperlink ref="B21" r:id="rId3" display="https://iopscience.iop.org/article/10.3847/1538-4357/ad150d/pdf" xr:uid="{2B29DA26-0CAF-4134-8DB4-81B7FB248206}"/>
+    <hyperlink ref="B23" r:id="rId2" display="https://iopscience.iop.org/article/10.1088/0004-637X/792/2/134/pdf" xr:uid="{61E00B74-8AA3-4F56-8D64-5040CF6273FD}"/>
+    <hyperlink ref="B24" r:id="rId3" display="https://iopscience.iop.org/article/10.3847/1538-4357/ad150d/pdf" xr:uid="{2B29DA26-0CAF-4134-8DB4-81B7FB248206}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://iopscience.iop.org/article/10.3847/1538-4357/aaa45a/pdf" xr:uid="{6356AD82-CED8-4181-BE88-E495BE2AB77F}"/>
     <hyperlink ref="B8" r:id="rId5" xr:uid="{17CDB83C-EA18-4DA4-B461-3A04D1F396BC}"/>
+    <hyperlink ref="B13" r:id="rId6" display="https://iopscience.iop.org/article/10.3847/2041-8213/ab9df5/pdf" xr:uid="{30496D10-F953-4D31-9A96-C44C6AB4C76A}"/>
+    <hyperlink ref="B15" r:id="rId7" location="ajab94a7f3" display="https://iopscience.iop.org/article/10.3847/1538-3881/ab94a7/meta - ajab94a7f3" xr:uid="{D9D0F3A4-9289-4F6C-9CC2-06E5108B5D94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to flowchart and lit review
</commit_message>
<xml_diff>
--- a/doc/voyager_lism_lit_review.xlsx
+++ b/doc/voyager_lism_lit_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spann\Documents\Research\Code repos\sf_gap_analysis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A310A-80D0-4DDC-8A8D-58CEE4C40B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2403FC2C-9137-4211-BC81-B84F155A9A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-2025" windowWidth="25440" windowHeight="15270" xr2:uid="{744BB5EC-7CDC-4C43-818F-74C8129A6F6E}"/>
+    <workbookView xWindow="20370" yWindow="-11385" windowWidth="29040" windowHeight="15720" xr2:uid="{744BB5EC-7CDC-4C43-818F-74C8129A6F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,7 +769,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>